<commit_message>
docs: updated remaining examples
</commit_message>
<xml_diff>
--- a/docs/artifacts/rules/dms-rebuild-olav.xlsx
+++ b/docs/artifacts/rules/dms-rebuild-olav.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\docs\artifacts\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4734D3A-88D6-47C1-BFFD-4003EAAB1615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF82E5C3-3981-4779-9A5F-F3E603EA7B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="264">
   <si>
     <t>role</t>
   </si>
@@ -820,6 +820,9 @@
   </si>
   <si>
     <t>power</t>
+  </si>
+  <si>
+    <t>Immutable</t>
   </si>
 </sst>
 </file>
@@ -2104,7 +2107,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -2214,11 +2217,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:P19"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J15" sqref="J15"/>
+      <selection pane="bottomLeft" activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2227,16 +2230,16 @@
     <col min="2" max="2" width="20.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="13" customWidth="1"/>
     <col min="6" max="6" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="59.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.44140625" customWidth="1"/>
-    <col min="13" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="14.44140625" customWidth="1"/>
-    <col min="16" max="16" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="13" customWidth="1"/>
+    <col min="11" max="11" width="59.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.44140625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
+    <col min="16" max="16" width="14.44140625" customWidth="1"/>
+    <col min="17" max="17" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:17" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
         <v>21</v>
       </c>
@@ -2255,8 +2258,9 @@
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
       <c r="P1" s="7"/>
-    </row>
-    <row r="2" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+      <c r="Q1" s="7"/>
+    </row>
+    <row r="2" spans="1:17" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
@@ -2279,34 +2283,37 @@
         <v>28</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>67</v>
       </c>
@@ -2327,24 +2334,27 @@
       <c r="H3" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I3" s="3"/>
+      <c r="I3" s="3" t="b">
+        <v>0</v>
+      </c>
       <c r="J3" s="3"/>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="3"/>
+      <c r="L3" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="M3" s="3"/>
       <c r="N3" s="3"/>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="3"/>
+      <c r="P3" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>67</v>
       </c>
@@ -2363,24 +2373,27 @@
       <c r="H4" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I4" s="3"/>
+      <c r="I4" s="3" t="b">
+        <v>0</v>
+      </c>
       <c r="J4" s="3"/>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="3"/>
+      <c r="L4" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="3"/>
       <c r="N4" s="3"/>
-      <c r="O4" s="3" t="s">
+      <c r="O4" s="3"/>
+      <c r="P4" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>67</v>
       </c>
@@ -2396,23 +2409,24 @@
         <v>53</v>
       </c>
       <c r="G5" s="3"/>
-      <c r="H5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
-      <c r="O5" s="3" t="s">
+      <c r="O5" s="3"/>
+      <c r="P5" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="Q5" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>67</v>
       </c>
@@ -2428,23 +2442,24 @@
         <v>53</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
-      <c r="O6" s="3" t="s">
+      <c r="O6" s="3"/>
+      <c r="P6" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="Q6" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>67</v>
       </c>
@@ -2465,26 +2480,29 @@
       <c r="H7" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4" t="s">
+      <c r="I7" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="L7" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="M7" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="M7" s="4"/>
       <c r="N7" s="4"/>
-      <c r="O7" s="4" t="s">
+      <c r="O7" s="4"/>
+      <c r="P7" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="P7" s="4" t="s">
+      <c r="Q7" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>67</v>
       </c>
@@ -2500,23 +2518,24 @@
         <v>76</v>
       </c>
       <c r="G8" s="3"/>
-      <c r="H8" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
-      <c r="O8" s="3" t="s">
+      <c r="O8" s="3"/>
+      <c r="P8" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="P8" s="3" t="s">
+      <c r="Q8" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -2533,8 +2552,9 @@
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q9" s="3"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>76</v>
       </c>
@@ -2553,24 +2573,27 @@
       <c r="H10" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I10" s="4"/>
+      <c r="I10" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J10" s="4"/>
-      <c r="K10" s="4" t="s">
+      <c r="K10" s="4"/>
+      <c r="L10" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="M10" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="M10" s="4"/>
       <c r="N10" s="4"/>
-      <c r="O10" s="4" t="s">
+      <c r="O10" s="4"/>
+      <c r="P10" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="P10" s="4" t="s">
+      <c r="Q10" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>76</v>
       </c>
@@ -2591,24 +2614,27 @@
       <c r="H11" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I11" s="4"/>
+      <c r="I11" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J11" s="4"/>
-      <c r="K11" s="4" t="s">
+      <c r="K11" s="4"/>
+      <c r="L11" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="L11" s="4" t="s">
+      <c r="M11" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="M11" s="4"/>
       <c r="N11" s="4"/>
-      <c r="O11" s="4" t="s">
+      <c r="O11" s="4"/>
+      <c r="P11" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="P11" s="4" t="s">
+      <c r="Q11" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>76</v>
       </c>
@@ -2627,24 +2653,27 @@
       <c r="H12" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I12" s="4"/>
+      <c r="I12" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J12" s="4"/>
-      <c r="K12" s="4" t="s">
+      <c r="K12" s="4"/>
+      <c r="L12" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="M12" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="M12" s="4"/>
       <c r="N12" s="4"/>
-      <c r="O12" s="4" t="s">
+      <c r="O12" s="4"/>
+      <c r="P12" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="P12" s="4" t="s">
+      <c r="Q12" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>76</v>
       </c>
@@ -2663,24 +2692,27 @@
       <c r="H13" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I13" s="4"/>
+      <c r="I13" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J13" s="4"/>
-      <c r="K13" s="4" t="s">
+      <c r="K13" s="4"/>
+      <c r="L13" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="L13" s="4" t="s">
+      <c r="M13" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="M13" s="4"/>
       <c r="N13" s="4"/>
-      <c r="O13" s="4" t="s">
+      <c r="O13" s="4"/>
+      <c r="P13" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="P13" s="4" t="s">
+      <c r="Q13" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>76</v>
       </c>
@@ -2699,24 +2731,27 @@
       <c r="H14" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I14" s="4"/>
+      <c r="I14" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J14" s="4"/>
-      <c r="K14" s="4" t="s">
+      <c r="K14" s="4"/>
+      <c r="L14" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="L14" s="4" t="s">
+      <c r="M14" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="M14" s="4"/>
       <c r="N14" s="4"/>
-      <c r="O14" s="4" t="s">
+      <c r="O14" s="4"/>
+      <c r="P14" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="P14" s="4" t="s">
+      <c r="Q14" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>76</v>
       </c>
@@ -2737,26 +2772,29 @@
       <c r="H15" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4" t="s">
+      <c r="I15" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="L15" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="L15" s="4" t="s">
+      <c r="M15" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="M15" s="4"/>
       <c r="N15" s="4"/>
-      <c r="O15" s="4" t="s">
+      <c r="O15" s="4"/>
+      <c r="P15" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="P15" s="4" t="s">
+      <c r="Q15" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>76</v>
       </c>
@@ -2775,24 +2813,27 @@
       <c r="H16" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I16" s="4"/>
+      <c r="I16" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J16" s="4"/>
-      <c r="K16" s="4" t="s">
+      <c r="K16" s="4"/>
+      <c r="L16" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="L16" s="4" t="s">
+      <c r="M16" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M16" s="4"/>
       <c r="N16" s="4"/>
-      <c r="O16" s="4" t="s">
+      <c r="O16" s="4"/>
+      <c r="P16" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="P16" s="4" t="s">
+      <c r="Q16" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>76</v>
       </c>
@@ -2808,23 +2849,24 @@
         <v>43</v>
       </c>
       <c r="G17" s="4"/>
-      <c r="H17" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
-      <c r="O17" s="4" t="s">
+      <c r="O17" s="4"/>
+      <c r="P17" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="P17" s="4" t="s">
+      <c r="Q17" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>76</v>
       </c>
@@ -2843,24 +2885,27 @@
       <c r="H18" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I18" s="4"/>
+      <c r="I18" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J18" s="4"/>
-      <c r="K18" s="4" t="s">
+      <c r="K18" s="4"/>
+      <c r="L18" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="L18" s="4" t="s">
+      <c r="M18" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="M18" s="4"/>
       <c r="N18" s="4"/>
-      <c r="O18" s="4" t="s">
+      <c r="O18" s="4"/>
+      <c r="P18" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="P18" s="4" t="s">
+      <c r="Q18" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>76</v>
       </c>
@@ -2879,26 +2924,29 @@
       <c r="H19" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I19" s="4"/>
+      <c r="I19" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J19" s="4"/>
-      <c r="K19" s="4" t="s">
+      <c r="K19" s="4"/>
+      <c r="L19" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="L19" s="4" t="s">
+      <c r="M19" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="M19" s="4"/>
       <c r="N19" s="4"/>
-      <c r="O19" s="4" t="s">
+      <c r="O19" s="4"/>
+      <c r="P19" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="P19" s="4" t="s">
+      <c r="Q19" s="4" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A1:Q1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -3118,11 +3166,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:P40"/>
+  <dimension ref="A1:Q40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3131,16 +3179,16 @@
     <col min="2" max="2" width="21.44140625" customWidth="1"/>
     <col min="3" max="5" width="13" customWidth="1"/>
     <col min="6" max="6" width="14.44140625" customWidth="1"/>
-    <col min="7" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="27.44140625" customWidth="1"/>
-    <col min="12" max="12" width="21.44140625" customWidth="1"/>
-    <col min="13" max="13" width="15.44140625" customWidth="1"/>
-    <col min="14" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="14.44140625" customWidth="1"/>
-    <col min="16" max="16" width="21.44140625" customWidth="1"/>
+    <col min="7" max="11" width="13" customWidth="1"/>
+    <col min="12" max="12" width="27.44140625" customWidth="1"/>
+    <col min="13" max="13" width="21.44140625" customWidth="1"/>
+    <col min="14" max="14" width="15.44140625" customWidth="1"/>
+    <col min="15" max="15" width="13" customWidth="1"/>
+    <col min="16" max="16" width="14.44140625" customWidth="1"/>
+    <col min="17" max="17" width="21.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:17" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
         <v>21</v>
       </c>
@@ -3159,8 +3207,9 @@
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
       <c r="P1" s="7"/>
-    </row>
-    <row r="2" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+      <c r="Q1" s="7"/>
+    </row>
+    <row r="2" spans="1:17" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
@@ -3183,34 +3232,37 @@
         <v>28</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>43</v>
       </c>
@@ -3229,26 +3281,29 @@
       <c r="H3" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I3" s="3"/>
+      <c r="I3" s="3" t="b">
+        <v>0</v>
+      </c>
       <c r="J3" s="3"/>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="3"/>
+      <c r="L3" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="3"/>
+      <c r="P3" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>43</v>
       </c>
@@ -3267,24 +3322,27 @@
       <c r="H4" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I4" s="3"/>
+      <c r="I4" s="3" t="b">
+        <v>0</v>
+      </c>
       <c r="J4" s="3"/>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="3"/>
+      <c r="L4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="M4" s="3"/>
       <c r="N4" s="3"/>
-      <c r="O4" s="3" t="s">
+      <c r="O4" s="3"/>
+      <c r="P4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>43</v>
       </c>
@@ -3301,26 +3359,29 @@
         <v>1</v>
       </c>
       <c r="H5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="I5" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="J5" s="3"/>
-      <c r="K5" s="3" t="s">
+      <c r="K5" s="3"/>
+      <c r="L5" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="M5" s="3"/>
       <c r="N5" s="3"/>
-      <c r="O5" s="3" t="s">
+      <c r="O5" s="3"/>
+      <c r="P5" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="Q5" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>43</v>
       </c>
@@ -3339,26 +3400,29 @@
       <c r="H6" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I6" s="3"/>
+      <c r="I6" s="3" t="b">
+        <v>0</v>
+      </c>
       <c r="J6" s="3"/>
-      <c r="K6" s="3" t="s">
+      <c r="K6" s="3"/>
+      <c r="L6" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3" t="s">
+      <c r="O6" s="3"/>
+      <c r="P6" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="Q6" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>43</v>
       </c>
@@ -3377,24 +3441,27 @@
       <c r="H7" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I7" s="3"/>
+      <c r="I7" s="3" t="b">
+        <v>0</v>
+      </c>
       <c r="J7" s="3"/>
-      <c r="K7" s="3" t="s">
+      <c r="K7" s="3"/>
+      <c r="L7" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="M7" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="M7" s="3"/>
       <c r="N7" s="3"/>
-      <c r="O7" s="3" t="s">
+      <c r="O7" s="3"/>
+      <c r="P7" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="P7" s="3" t="s">
+      <c r="Q7" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -3411,8 +3478,9 @@
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q8" s="3"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>53</v>
       </c>
@@ -3431,24 +3499,27 @@
       <c r="H9" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I9" s="4"/>
+      <c r="I9" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J9" s="4"/>
-      <c r="K9" s="4" t="s">
+      <c r="K9" s="4"/>
+      <c r="L9" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="M9" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="M9" s="4"/>
       <c r="N9" s="4"/>
-      <c r="O9" s="4" t="s">
+      <c r="O9" s="4"/>
+      <c r="P9" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="P9" s="4" t="s">
+      <c r="Q9" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>53</v>
       </c>
@@ -3467,24 +3538,27 @@
       <c r="H10" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I10" s="4"/>
+      <c r="I10" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J10" s="4"/>
-      <c r="K10" s="4" t="s">
+      <c r="K10" s="4"/>
+      <c r="L10" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="M10" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="M10" s="4"/>
       <c r="N10" s="4"/>
-      <c r="O10" s="4" t="s">
+      <c r="O10" s="4"/>
+      <c r="P10" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="P10" s="4" t="s">
+      <c r="Q10" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>53</v>
       </c>
@@ -3503,24 +3577,27 @@
       <c r="H11" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I11" s="4"/>
+      <c r="I11" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J11" s="4"/>
-      <c r="K11" s="4" t="s">
+      <c r="K11" s="4"/>
+      <c r="L11" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="L11" s="4" t="s">
+      <c r="M11" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="M11" s="4"/>
       <c r="N11" s="4"/>
-      <c r="O11" s="4" t="s">
+      <c r="O11" s="4"/>
+      <c r="P11" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="P11" s="4" t="s">
+      <c r="Q11" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>53</v>
       </c>
@@ -3541,24 +3618,27 @@
       <c r="H12" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I12" s="4"/>
+      <c r="I12" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J12" s="4"/>
-      <c r="K12" s="4" t="s">
+      <c r="K12" s="4"/>
+      <c r="L12" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="M12" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="M12" s="4"/>
       <c r="N12" s="4"/>
-      <c r="O12" s="4" t="s">
+      <c r="O12" s="4"/>
+      <c r="P12" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="P12" s="4" t="s">
+      <c r="Q12" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>53</v>
       </c>
@@ -3577,26 +3657,29 @@
       <c r="H13" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I13" s="4"/>
+      <c r="I13" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J13" s="4"/>
-      <c r="K13" s="4" t="s">
+      <c r="K13" s="4"/>
+      <c r="L13" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="L13" s="4" t="s">
+      <c r="M13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M13" s="4" t="s">
+      <c r="N13" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4" t="s">
+      <c r="O13" s="4"/>
+      <c r="P13" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="P13" s="4" t="s">
+      <c r="Q13" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>53</v>
       </c>
@@ -3615,24 +3698,27 @@
       <c r="H14" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I14" s="4"/>
+      <c r="I14" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J14" s="4"/>
-      <c r="K14" s="4" t="s">
+      <c r="K14" s="4"/>
+      <c r="L14" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="L14" s="4" t="s">
+      <c r="M14" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="M14" s="4"/>
       <c r="N14" s="4"/>
-      <c r="O14" s="4" t="s">
+      <c r="O14" s="4"/>
+      <c r="P14" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="P14" s="4" t="s">
+      <c r="Q14" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>53</v>
       </c>
@@ -3651,26 +3737,29 @@
       <c r="H15" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I15" s="4"/>
+      <c r="I15" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J15" s="4"/>
-      <c r="K15" s="4" t="s">
+      <c r="K15" s="4"/>
+      <c r="L15" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="L15" s="4" t="s">
+      <c r="M15" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="M15" s="4" t="s">
+      <c r="N15" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4" t="s">
+      <c r="O15" s="4"/>
+      <c r="P15" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="P15" s="4" t="s">
+      <c r="Q15" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>53</v>
       </c>
@@ -3689,26 +3778,29 @@
       <c r="H16" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I16" s="4"/>
+      <c r="I16" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J16" s="4"/>
-      <c r="K16" s="4" t="s">
+      <c r="K16" s="4"/>
+      <c r="L16" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="L16" s="4" t="s">
+      <c r="M16" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="M16" s="4" t="s">
+      <c r="N16" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4" t="s">
+      <c r="O16" s="4"/>
+      <c r="P16" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="P16" s="4" t="s">
+      <c r="Q16" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>53</v>
       </c>
@@ -3727,24 +3819,27 @@
       <c r="H17" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I17" s="4"/>
+      <c r="I17" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J17" s="4"/>
-      <c r="K17" s="4" t="s">
+      <c r="K17" s="4"/>
+      <c r="L17" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="L17" s="4" t="s">
+      <c r="M17" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="M17" s="4"/>
       <c r="N17" s="4"/>
-      <c r="O17" s="4" t="s">
+      <c r="O17" s="4"/>
+      <c r="P17" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="P17" s="4" t="s">
+      <c r="Q17" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>53</v>
       </c>
@@ -3763,24 +3858,27 @@
       <c r="H18" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I18" s="4"/>
+      <c r="I18" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J18" s="4"/>
-      <c r="K18" s="4" t="s">
+      <c r="K18" s="4"/>
+      <c r="L18" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="L18" s="4" t="s">
+      <c r="M18" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="M18" s="4"/>
       <c r="N18" s="4"/>
-      <c r="O18" s="4" t="s">
+      <c r="O18" s="4"/>
+      <c r="P18" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="P18" s="4" t="s">
+      <c r="Q18" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -3797,8 +3895,9 @@
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q19" s="4"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>67</v>
       </c>
@@ -3817,24 +3916,27 @@
       <c r="H20" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I20" s="3"/>
+      <c r="I20" s="3" t="b">
+        <v>0</v>
+      </c>
       <c r="J20" s="3"/>
-      <c r="K20" s="3" t="s">
+      <c r="K20" s="3"/>
+      <c r="L20" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="L20" s="3" t="s">
+      <c r="M20" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="M20" s="3"/>
       <c r="N20" s="3"/>
-      <c r="O20" s="3" t="s">
+      <c r="O20" s="3"/>
+      <c r="P20" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="P20" s="3" t="s">
+      <c r="Q20" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>67</v>
       </c>
@@ -3855,24 +3957,27 @@
       <c r="H21" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I21" s="3"/>
+      <c r="I21" s="3" t="b">
+        <v>0</v>
+      </c>
       <c r="J21" s="3"/>
-      <c r="K21" s="3" t="s">
+      <c r="K21" s="3"/>
+      <c r="L21" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="L21" s="3" t="s">
+      <c r="M21" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="M21" s="3"/>
       <c r="N21" s="3"/>
-      <c r="O21" s="3" t="s">
+      <c r="O21" s="3"/>
+      <c r="P21" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="P21" s="3" t="s">
+      <c r="Q21" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>67</v>
       </c>
@@ -3891,24 +3996,27 @@
       <c r="H22" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I22" s="3"/>
+      <c r="I22" s="3" t="b">
+        <v>0</v>
+      </c>
       <c r="J22" s="3"/>
-      <c r="K22" s="3" t="s">
+      <c r="K22" s="3"/>
+      <c r="L22" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="L22" s="3" t="s">
+      <c r="M22" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="M22" s="3"/>
       <c r="N22" s="3"/>
-      <c r="O22" s="3" t="s">
+      <c r="O22" s="3"/>
+      <c r="P22" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="P22" s="3" t="s">
+      <c r="Q22" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>67</v>
       </c>
@@ -3927,24 +4035,27 @@
       <c r="H23" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I23" s="3"/>
+      <c r="I23" s="3" t="b">
+        <v>0</v>
+      </c>
       <c r="J23" s="3"/>
-      <c r="K23" s="3" t="s">
+      <c r="K23" s="3"/>
+      <c r="L23" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="L23" s="3" t="s">
+      <c r="M23" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="M23" s="3"/>
       <c r="N23" s="3"/>
-      <c r="O23" s="3" t="s">
+      <c r="O23" s="3"/>
+      <c r="P23" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="P23" s="3" t="s">
+      <c r="Q23" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>67</v>
       </c>
@@ -3963,24 +4074,27 @@
       <c r="H24" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I24" s="3"/>
+      <c r="I24" s="3" t="b">
+        <v>0</v>
+      </c>
       <c r="J24" s="3"/>
-      <c r="K24" s="3" t="s">
+      <c r="K24" s="3"/>
+      <c r="L24" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="L24" s="3" t="s">
+      <c r="M24" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M24" s="3"/>
       <c r="N24" s="3"/>
-      <c r="O24" s="3" t="s">
+      <c r="O24" s="3"/>
+      <c r="P24" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="P24" s="3" t="s">
+      <c r="Q24" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>67</v>
       </c>
@@ -3996,23 +4110,24 @@
         <v>53</v>
       </c>
       <c r="G25" s="3"/>
-      <c r="H25" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
-      <c r="O25" s="3" t="s">
+      <c r="O25" s="3"/>
+      <c r="P25" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="P25" s="3" t="s">
+      <c r="Q25" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>67</v>
       </c>
@@ -4028,23 +4143,24 @@
         <v>53</v>
       </c>
       <c r="G26" s="3"/>
-      <c r="H26" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
-      <c r="O26" s="3" t="s">
+      <c r="O26" s="3"/>
+      <c r="P26" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="P26" s="3" t="s">
+      <c r="Q26" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>67</v>
       </c>
@@ -4060,23 +4176,24 @@
         <v>76</v>
       </c>
       <c r="G27" s="3"/>
-      <c r="H27" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
-      <c r="O27" s="3" t="s">
+      <c r="O27" s="3"/>
+      <c r="P27" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="P27" s="3" t="s">
+      <c r="Q27" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -4093,8 +4210,9 @@
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
       <c r="P28" s="3"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q28" s="3"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>76</v>
       </c>
@@ -4113,24 +4231,27 @@
       <c r="H29" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I29" s="4"/>
+      <c r="I29" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J29" s="4"/>
-      <c r="K29" s="4" t="s">
+      <c r="K29" s="4"/>
+      <c r="L29" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="L29" s="4" t="s">
+      <c r="M29" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="M29" s="4"/>
       <c r="N29" s="4"/>
-      <c r="O29" s="4" t="s">
+      <c r="O29" s="4"/>
+      <c r="P29" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="P29" s="4" t="s">
+      <c r="Q29" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>76</v>
       </c>
@@ -4151,24 +4272,27 @@
       <c r="H30" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I30" s="4"/>
+      <c r="I30" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J30" s="4"/>
-      <c r="K30" s="4" t="s">
+      <c r="K30" s="4"/>
+      <c r="L30" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="L30" s="4" t="s">
+      <c r="M30" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="M30" s="4"/>
       <c r="N30" s="4"/>
-      <c r="O30" s="4" t="s">
+      <c r="O30" s="4"/>
+      <c r="P30" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="P30" s="4" t="s">
+      <c r="Q30" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>76</v>
       </c>
@@ -4187,24 +4311,27 @@
       <c r="H31" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I31" s="4"/>
+      <c r="I31" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J31" s="4"/>
-      <c r="K31" s="4" t="s">
+      <c r="K31" s="4"/>
+      <c r="L31" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="L31" s="4" t="s">
+      <c r="M31" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="M31" s="4"/>
       <c r="N31" s="4"/>
-      <c r="O31" s="4" t="s">
+      <c r="O31" s="4"/>
+      <c r="P31" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="P31" s="4" t="s">
+      <c r="Q31" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>76</v>
       </c>
@@ -4223,24 +4350,27 @@
       <c r="H32" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I32" s="4"/>
+      <c r="I32" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J32" s="4"/>
-      <c r="K32" s="4" t="s">
+      <c r="K32" s="4"/>
+      <c r="L32" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="L32" s="4" t="s">
+      <c r="M32" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="M32" s="4"/>
       <c r="N32" s="4"/>
-      <c r="O32" s="4" t="s">
+      <c r="O32" s="4"/>
+      <c r="P32" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="P32" s="4" t="s">
+      <c r="Q32" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>76</v>
       </c>
@@ -4259,24 +4389,27 @@
       <c r="H33" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I33" s="4"/>
+      <c r="I33" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J33" s="4"/>
-      <c r="K33" s="4" t="s">
+      <c r="K33" s="4"/>
+      <c r="L33" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="L33" s="4" t="s">
+      <c r="M33" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="M33" s="4"/>
       <c r="N33" s="4"/>
-      <c r="O33" s="4" t="s">
+      <c r="O33" s="4"/>
+      <c r="P33" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="P33" s="4" t="s">
+      <c r="Q33" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>76</v>
       </c>
@@ -4295,24 +4428,27 @@
       <c r="H34" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I34" s="4"/>
+      <c r="I34" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J34" s="4"/>
-      <c r="K34" s="4" t="s">
+      <c r="K34" s="4"/>
+      <c r="L34" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="L34" s="4" t="s">
+      <c r="M34" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="M34" s="4"/>
       <c r="N34" s="4"/>
-      <c r="O34" s="4" t="s">
+      <c r="O34" s="4"/>
+      <c r="P34" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="P34" s="4" t="s">
+      <c r="Q34" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>76</v>
       </c>
@@ -4331,24 +4467,27 @@
       <c r="H35" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I35" s="4"/>
+      <c r="I35" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J35" s="4"/>
-      <c r="K35" s="4" t="s">
+      <c r="K35" s="4"/>
+      <c r="L35" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="L35" s="4" t="s">
+      <c r="M35" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="M35" s="4"/>
       <c r="N35" s="4"/>
-      <c r="O35" s="4" t="s">
+      <c r="O35" s="4"/>
+      <c r="P35" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="P35" s="4" t="s">
+      <c r="Q35" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>76</v>
       </c>
@@ -4367,24 +4506,27 @@
       <c r="H36" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I36" s="4"/>
+      <c r="I36" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J36" s="4"/>
-      <c r="K36" s="4" t="s">
+      <c r="K36" s="4"/>
+      <c r="L36" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="L36" s="4" t="s">
+      <c r="M36" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="M36" s="4"/>
       <c r="N36" s="4"/>
-      <c r="O36" s="4" t="s">
+      <c r="O36" s="4"/>
+      <c r="P36" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="P36" s="4" t="s">
+      <c r="Q36" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>76</v>
       </c>
@@ -4403,24 +4545,27 @@
       <c r="H37" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I37" s="4"/>
+      <c r="I37" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J37" s="4"/>
-      <c r="K37" s="4" t="s">
+      <c r="K37" s="4"/>
+      <c r="L37" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="L37" s="4" t="s">
+      <c r="M37" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M37" s="4"/>
       <c r="N37" s="4"/>
-      <c r="O37" s="4" t="s">
+      <c r="O37" s="4"/>
+      <c r="P37" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="P37" s="4" t="s">
+      <c r="Q37" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>76</v>
       </c>
@@ -4436,23 +4581,24 @@
         <v>43</v>
       </c>
       <c r="G38" s="4"/>
-      <c r="H38" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
       <c r="N38" s="4"/>
-      <c r="O38" s="4" t="s">
+      <c r="O38" s="4"/>
+      <c r="P38" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="P38" s="4" t="s">
+      <c r="Q38" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>76</v>
       </c>
@@ -4471,24 +4617,27 @@
       <c r="H39" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I39" s="4"/>
+      <c r="I39" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J39" s="4"/>
-      <c r="K39" s="4" t="s">
+      <c r="K39" s="4"/>
+      <c r="L39" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="L39" s="4" t="s">
+      <c r="M39" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="M39" s="4"/>
       <c r="N39" s="4"/>
-      <c r="O39" s="4" t="s">
+      <c r="O39" s="4"/>
+      <c r="P39" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="P39" s="4" t="s">
+      <c r="Q39" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>76</v>
       </c>
@@ -4507,26 +4656,29 @@
       <c r="H40" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I40" s="4"/>
+      <c r="I40" s="4" t="b">
+        <v>0</v>
+      </c>
       <c r="J40" s="4"/>
-      <c r="K40" s="4" t="s">
+      <c r="K40" s="4"/>
+      <c r="L40" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="L40" s="4" t="s">
+      <c r="M40" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="M40" s="4"/>
       <c r="N40" s="4"/>
-      <c r="O40" s="4" t="s">
+      <c r="O40" s="4"/>
+      <c r="P40" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="P40" s="4" t="s">
+      <c r="Q40" s="4" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A1:Q1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -4868,11 +5020,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:P75"/>
+  <dimension ref="A1:Q75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G77" sqref="G77"/>
+      <selection pane="bottomLeft" activeCell="H68" sqref="H68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4881,16 +5033,16 @@
     <col min="2" max="2" width="20.44140625" customWidth="1"/>
     <col min="3" max="5" width="13" customWidth="1"/>
     <col min="6" max="6" width="25.44140625" customWidth="1"/>
-    <col min="7" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="74.44140625" customWidth="1"/>
-    <col min="11" max="11" width="38.44140625" customWidth="1"/>
-    <col min="12" max="12" width="20.44140625" customWidth="1"/>
-    <col min="13" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="25.44140625" customWidth="1"/>
-    <col min="16" max="16" width="20.44140625" customWidth="1"/>
+    <col min="7" max="10" width="13" customWidth="1"/>
+    <col min="11" max="11" width="74.44140625" customWidth="1"/>
+    <col min="12" max="12" width="38.44140625" customWidth="1"/>
+    <col min="13" max="13" width="20.44140625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
+    <col min="16" max="16" width="25.44140625" customWidth="1"/>
+    <col min="17" max="17" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:17" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="6" t="s">
         <v>21</v>
       </c>
@@ -4909,8 +5061,9 @@
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
       <c r="P1" s="7"/>
-    </row>
-    <row r="2" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+      <c r="Q1" s="7"/>
+    </row>
+    <row r="2" spans="1:17" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
@@ -4933,34 +5086,37 @@
         <v>28</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>90</v>
       </c>
@@ -4979,26 +5135,29 @@
       <c r="H3" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3" t="s">
+      <c r="I3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="M3" s="3"/>
       <c r="N3" s="3"/>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="3"/>
+      <c r="P3" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -5015,8 +5174,9 @@
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q4" s="3"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>92</v>
       </c>
@@ -5035,26 +5195,29 @@
       <c r="H5" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4" t="s">
+      <c r="I5" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="L5" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="M5" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="M5" s="4"/>
       <c r="N5" s="4"/>
-      <c r="O5" s="4" t="s">
+      <c r="O5" s="4"/>
+      <c r="P5" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="Q5" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -5071,8 +5234,9 @@
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q6" s="4"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>93</v>
       </c>
@@ -5091,26 +5255,29 @@
       <c r="H7" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3" t="s">
+      <c r="I7" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="L7" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="M7" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="M7" s="3"/>
       <c r="N7" s="3"/>
-      <c r="O7" s="3" t="s">
+      <c r="O7" s="3"/>
+      <c r="P7" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="P7" s="3" t="s">
+      <c r="Q7" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -5127,8 +5294,9 @@
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q8" s="3"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>94</v>
       </c>
@@ -5147,26 +5315,29 @@
       <c r="H9" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4" t="s">
+      <c r="I9" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="L9" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="L9" s="4" t="s">
+      <c r="M9" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="M9" s="4"/>
       <c r="N9" s="4"/>
-      <c r="O9" s="4" t="s">
+      <c r="O9" s="4"/>
+      <c r="P9" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="P9" s="4" t="s">
+      <c r="Q9" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>94</v>
       </c>
@@ -5187,26 +5358,29 @@
       <c r="H10" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4" t="s">
+      <c r="I10" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="L10" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="M10" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="M10" s="4"/>
       <c r="N10" s="4"/>
-      <c r="O10" s="4" t="s">
+      <c r="O10" s="4"/>
+      <c r="P10" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="P10" s="4" t="s">
+      <c r="Q10" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>94</v>
       </c>
@@ -5225,26 +5399,29 @@
       <c r="H11" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4" t="s">
+      <c r="I11" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="L11" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="L11" s="4" t="s">
+      <c r="M11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M11" s="4"/>
       <c r="N11" s="4"/>
-      <c r="O11" s="4" t="s">
+      <c r="O11" s="4"/>
+      <c r="P11" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="P11" s="4" t="s">
+      <c r="Q11" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>94</v>
       </c>
@@ -5265,26 +5442,29 @@
       <c r="H12" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4" t="s">
+      <c r="I12" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="L12" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="M12" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="M12" s="4"/>
       <c r="N12" s="4"/>
-      <c r="O12" s="4" t="s">
+      <c r="O12" s="4"/>
+      <c r="P12" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="P12" s="4" t="s">
+      <c r="Q12" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>94</v>
       </c>
@@ -5303,26 +5483,29 @@
       <c r="H13" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4" t="s">
+      <c r="I13" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="K13" s="4" t="s">
+      <c r="L13" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="L13" s="4" t="s">
+      <c r="M13" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="M13" s="4"/>
       <c r="N13" s="4"/>
-      <c r="O13" s="4" t="s">
+      <c r="O13" s="4"/>
+      <c r="P13" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="P13" s="4" t="s">
+      <c r="Q13" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -5339,8 +5522,9 @@
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q14" s="4"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>97</v>
       </c>
@@ -5359,26 +5543,29 @@
       <c r="H15" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3" t="s">
+      <c r="I15" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="K15" s="3" t="s">
+      <c r="L15" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="L15" s="3" t="s">
+      <c r="M15" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="M15" s="3"/>
       <c r="N15" s="3"/>
-      <c r="O15" s="3" t="s">
+      <c r="O15" s="3"/>
+      <c r="P15" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="P15" s="3" t="s">
+      <c r="Q15" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>97</v>
       </c>
@@ -5399,26 +5586,29 @@
       <c r="H16" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3" t="s">
+      <c r="I16" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="K16" s="3" t="s">
+      <c r="L16" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="L16" s="3" t="s">
+      <c r="M16" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="M16" s="3"/>
       <c r="N16" s="3"/>
-      <c r="O16" s="3" t="s">
+      <c r="O16" s="3"/>
+      <c r="P16" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="P16" s="3" t="s">
+      <c r="Q16" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>97</v>
       </c>
@@ -5437,26 +5627,29 @@
       <c r="H17" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3" t="s">
+      <c r="I17" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="K17" s="3" t="s">
+      <c r="L17" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="L17" s="3" t="s">
+      <c r="M17" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M17" s="3"/>
       <c r="N17" s="3"/>
-      <c r="O17" s="3" t="s">
+      <c r="O17" s="3"/>
+      <c r="P17" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="P17" s="3" t="s">
+      <c r="Q17" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -5473,8 +5666,9 @@
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q18" s="3"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>100</v>
       </c>
@@ -5493,26 +5687,29 @@
       <c r="H19" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4" t="s">
+      <c r="I19" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="K19" s="4" t="s">
+      <c r="L19" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="L19" s="4" t="s">
+      <c r="M19" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="M19" s="4"/>
       <c r="N19" s="4"/>
-      <c r="O19" s="4" t="s">
+      <c r="O19" s="4"/>
+      <c r="P19" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="P19" s="4" t="s">
+      <c r="Q19" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>100</v>
       </c>
@@ -5533,26 +5730,29 @@
       <c r="H20" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4" t="s">
+      <c r="I20" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="K20" s="4" t="s">
+      <c r="L20" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="L20" s="4" t="s">
+      <c r="M20" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="M20" s="4"/>
       <c r="N20" s="4"/>
-      <c r="O20" s="4" t="s">
+      <c r="O20" s="4"/>
+      <c r="P20" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="P20" s="4" t="s">
+      <c r="Q20" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>100</v>
       </c>
@@ -5571,26 +5771,29 @@
       <c r="H21" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4" t="s">
+      <c r="I21" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="K21" s="4" t="s">
+      <c r="L21" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="L21" s="4" t="s">
+      <c r="M21" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M21" s="4"/>
       <c r="N21" s="4"/>
-      <c r="O21" s="4" t="s">
+      <c r="O21" s="4"/>
+      <c r="P21" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="P21" s="4" t="s">
+      <c r="Q21" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>100</v>
       </c>
@@ -5611,26 +5814,29 @@
       <c r="H22" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4" t="s">
+      <c r="I22" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="K22" s="4" t="s">
+      <c r="L22" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="L22" s="4" t="s">
+      <c r="M22" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="M22" s="4"/>
       <c r="N22" s="4"/>
-      <c r="O22" s="4" t="s">
+      <c r="O22" s="4"/>
+      <c r="P22" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="P22" s="4" t="s">
+      <c r="Q22" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>100</v>
       </c>
@@ -5649,26 +5855,29 @@
       <c r="H23" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4" t="s">
+      <c r="I23" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="K23" s="4" t="s">
+      <c r="L23" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="L23" s="4" t="s">
+      <c r="M23" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="M23" s="4"/>
       <c r="N23" s="4"/>
-      <c r="O23" s="4" t="s">
+      <c r="O23" s="4"/>
+      <c r="P23" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="P23" s="4" t="s">
+      <c r="Q23" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -5685,8 +5894,9 @@
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q24" s="4"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>101</v>
       </c>
@@ -5705,26 +5915,29 @@
       <c r="H25" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3" t="s">
+      <c r="I25" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="K25" s="3" t="s">
+      <c r="L25" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="L25" s="3" t="s">
+      <c r="M25" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M25" s="3"/>
       <c r="N25" s="3"/>
-      <c r="O25" s="3" t="s">
+      <c r="O25" s="3"/>
+      <c r="P25" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="P25" s="3" t="s">
+      <c r="Q25" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -5741,8 +5954,9 @@
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q26" s="3"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>102</v>
       </c>
@@ -5758,25 +5972,26 @@
         <v>104</v>
       </c>
       <c r="G27" s="4"/>
-      <c r="H27" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4" t="s">
+      <c r="H27" s="4"/>
+      <c r="I27" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="K27" s="4"/>
       <c r="L27" s="4"/>
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
-      <c r="O27" s="4" t="s">
+      <c r="O27" s="4"/>
+      <c r="P27" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="P27" s="4" t="s">
+      <c r="Q27" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>102</v>
       </c>
@@ -5795,26 +6010,29 @@
       <c r="H28" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4" t="s">
+      <c r="I28" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="K28" s="4" t="s">
+      <c r="L28" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="L28" s="4" t="s">
+      <c r="M28" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="M28" s="4"/>
       <c r="N28" s="4"/>
-      <c r="O28" s="4" t="s">
+      <c r="O28" s="4"/>
+      <c r="P28" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="P28" s="4" t="s">
+      <c r="Q28" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>102</v>
       </c>
@@ -5835,26 +6053,29 @@
       <c r="H29" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4" t="s">
+      <c r="I29" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="K29" s="4" t="s">
+      <c r="L29" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="L29" s="4" t="s">
+      <c r="M29" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="M29" s="4"/>
       <c r="N29" s="4"/>
-      <c r="O29" s="4" t="s">
+      <c r="O29" s="4"/>
+      <c r="P29" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="P29" s="4" t="s">
+      <c r="Q29" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -5871,8 +6092,9 @@
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q30" s="4"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>108</v>
       </c>
@@ -5888,25 +6110,26 @@
         <v>59</v>
       </c>
       <c r="G31" s="3"/>
-      <c r="H31" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3" t="s">
+      <c r="H31" s="3"/>
+      <c r="I31" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="K31" s="3"/>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
-      <c r="O31" s="3" t="s">
+      <c r="O31" s="3"/>
+      <c r="P31" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="P31" s="3" t="s">
+      <c r="Q31" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -5923,8 +6146,9 @@
       <c r="N32" s="3"/>
       <c r="O32" s="3"/>
       <c r="P32" s="3"/>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q32" s="3"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>59</v>
       </c>
@@ -5943,26 +6167,29 @@
       <c r="H33" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4" t="s">
+      <c r="I33" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="K33" s="4" t="s">
+      <c r="L33" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="L33" s="4" t="s">
+      <c r="M33" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="M33" s="4"/>
       <c r="N33" s="4"/>
-      <c r="O33" s="4" t="s">
+      <c r="O33" s="4"/>
+      <c r="P33" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="P33" s="4" t="s">
+      <c r="Q33" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>59</v>
       </c>
@@ -5981,26 +6208,29 @@
       <c r="H34" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4" t="s">
+      <c r="I34" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="K34" s="4" t="s">
+      <c r="L34" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="L34" s="4" t="s">
+      <c r="M34" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="M34" s="4"/>
       <c r="N34" s="4"/>
-      <c r="O34" s="4" t="s">
+      <c r="O34" s="4"/>
+      <c r="P34" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="P34" s="4" t="s">
+      <c r="Q34" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -6017,8 +6247,9 @@
       <c r="N35" s="4"/>
       <c r="O35" s="4"/>
       <c r="P35" s="4"/>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q35" s="4"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>69</v>
       </c>
@@ -6034,25 +6265,26 @@
         <v>59</v>
       </c>
       <c r="G36" s="3"/>
-      <c r="H36" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3" t="s">
+      <c r="H36" s="3"/>
+      <c r="I36" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="K36" s="3"/>
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
       <c r="N36" s="3"/>
-      <c r="O36" s="3" t="s">
+      <c r="O36" s="3"/>
+      <c r="P36" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="P36" s="3" t="s">
+      <c r="Q36" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -6069,8 +6301,9 @@
       <c r="N37" s="3"/>
       <c r="O37" s="3"/>
       <c r="P37" s="3"/>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q37" s="3"/>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>112</v>
       </c>
@@ -6089,26 +6322,29 @@
       <c r="H38" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4" t="s">
+      <c r="I38" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="K38" s="4" t="s">
+      <c r="L38" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="L38" s="4" t="s">
+      <c r="M38" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="M38" s="4"/>
       <c r="N38" s="4"/>
-      <c r="O38" s="4" t="s">
+      <c r="O38" s="4"/>
+      <c r="P38" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="P38" s="4" t="s">
+      <c r="Q38" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>112</v>
       </c>
@@ -6129,26 +6365,29 @@
       <c r="H39" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4" t="s">
+      <c r="I39" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="K39" s="4" t="s">
+      <c r="L39" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="L39" s="4" t="s">
+      <c r="M39" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="M39" s="4"/>
       <c r="N39" s="4"/>
-      <c r="O39" s="4" t="s">
+      <c r="O39" s="4"/>
+      <c r="P39" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="P39" s="4" t="s">
+      <c r="Q39" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>112</v>
       </c>
@@ -6167,26 +6406,29 @@
       <c r="H40" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I40" s="4"/>
-      <c r="J40" s="4" t="s">
+      <c r="I40" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="K40" s="4" t="s">
+      <c r="L40" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="L40" s="4" t="s">
+      <c r="M40" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="M40" s="4"/>
       <c r="N40" s="4"/>
-      <c r="O40" s="4" t="s">
+      <c r="O40" s="4"/>
+      <c r="P40" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="P40" s="4" t="s">
+      <c r="Q40" s="4" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>112</v>
       </c>
@@ -6207,26 +6449,29 @@
       <c r="H41" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I41" s="4"/>
-      <c r="J41" s="4" t="s">
+      <c r="I41" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="K41" s="4" t="s">
+      <c r="L41" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="L41" s="4" t="s">
+      <c r="M41" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="M41" s="4"/>
       <c r="N41" s="4"/>
-      <c r="O41" s="4" t="s">
+      <c r="O41" s="4"/>
+      <c r="P41" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="P41" s="4" t="s">
+      <c r="Q41" s="4" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -6243,8 +6488,9 @@
       <c r="N42" s="4"/>
       <c r="O42" s="4"/>
       <c r="P42" s="4"/>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q42" s="4"/>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>117</v>
       </c>
@@ -6260,25 +6506,26 @@
         <v>90</v>
       </c>
       <c r="G43" s="3"/>
-      <c r="H43" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3" t="s">
+      <c r="H43" s="3"/>
+      <c r="I43" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="K43" s="3"/>
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
       <c r="N43" s="3"/>
-      <c r="O43" s="3" t="s">
+      <c r="O43" s="3"/>
+      <c r="P43" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="P43" s="3" t="s">
+      <c r="Q43" s="3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>117</v>
       </c>
@@ -6294,25 +6541,26 @@
         <v>92</v>
       </c>
       <c r="G44" s="3"/>
-      <c r="H44" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3" t="s">
+      <c r="H44" s="3"/>
+      <c r="I44" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="K44" s="3"/>
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
       <c r="N44" s="3"/>
-      <c r="O44" s="3" t="s">
+      <c r="O44" s="3"/>
+      <c r="P44" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="P44" s="3" t="s">
+      <c r="Q44" s="3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>117</v>
       </c>
@@ -6328,25 +6576,26 @@
         <v>93</v>
       </c>
       <c r="G45" s="3"/>
-      <c r="H45" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I45" s="3"/>
-      <c r="J45" s="3" t="s">
+      <c r="H45" s="3"/>
+      <c r="I45" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="K45" s="3"/>
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
       <c r="N45" s="3"/>
-      <c r="O45" s="3" t="s">
+      <c r="O45" s="3"/>
+      <c r="P45" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="P45" s="3" t="s">
+      <c r="Q45" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>117</v>
       </c>
@@ -6365,26 +6614,29 @@
       <c r="H46" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3" t="s">
+      <c r="I46" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="K46" s="3" t="s">
+      <c r="L46" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="L46" s="3" t="s">
+      <c r="M46" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="M46" s="3"/>
       <c r="N46" s="3"/>
-      <c r="O46" s="3" t="s">
+      <c r="O46" s="3"/>
+      <c r="P46" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="P46" s="3" t="s">
+      <c r="Q46" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>117</v>
       </c>
@@ -6405,26 +6657,29 @@
       <c r="H47" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3" t="s">
+      <c r="I47" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="K47" s="3" t="s">
+      <c r="L47" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="L47" s="3" t="s">
+      <c r="M47" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="M47" s="3"/>
       <c r="N47" s="3"/>
-      <c r="O47" s="3" t="s">
+      <c r="O47" s="3"/>
+      <c r="P47" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="P47" s="3" t="s">
+      <c r="Q47" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>117</v>
       </c>
@@ -6443,26 +6698,29 @@
       <c r="H48" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3" t="s">
+      <c r="I48" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J48" s="3"/>
+      <c r="K48" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="K48" s="3" t="s">
+      <c r="L48" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="L48" s="3" t="s">
+      <c r="M48" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M48" s="3"/>
       <c r="N48" s="3"/>
-      <c r="O48" s="3" t="s">
+      <c r="O48" s="3"/>
+      <c r="P48" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="P48" s="3" t="s">
+      <c r="Q48" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>117</v>
       </c>
@@ -6483,26 +6741,29 @@
       <c r="H49" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3" t="s">
+      <c r="I49" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J49" s="3"/>
+      <c r="K49" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="K49" s="3" t="s">
+      <c r="L49" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="L49" s="3" t="s">
+      <c r="M49" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="M49" s="3"/>
       <c r="N49" s="3"/>
-      <c r="O49" s="3" t="s">
+      <c r="O49" s="3"/>
+      <c r="P49" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="P49" s="3" t="s">
+      <c r="Q49" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>117</v>
       </c>
@@ -6521,26 +6782,29 @@
       <c r="H50" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3" t="s">
+      <c r="I50" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J50" s="3"/>
+      <c r="K50" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="K50" s="3" t="s">
+      <c r="L50" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="L50" s="3" t="s">
+      <c r="M50" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="M50" s="3"/>
       <c r="N50" s="3"/>
-      <c r="O50" s="3" t="s">
+      <c r="O50" s="3"/>
+      <c r="P50" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="P50" s="3" t="s">
+      <c r="Q50" s="3" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>117</v>
       </c>
@@ -6561,26 +6825,29 @@
       <c r="H51" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3" t="s">
+      <c r="I51" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J51" s="3"/>
+      <c r="K51" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="K51" s="3" t="s">
+      <c r="L51" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="L51" s="3" t="s">
+      <c r="M51" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="M51" s="3"/>
       <c r="N51" s="3"/>
-      <c r="O51" s="3" t="s">
+      <c r="O51" s="3"/>
+      <c r="P51" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="P51" s="3" t="s">
+      <c r="Q51" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>117</v>
       </c>
@@ -6599,26 +6866,29 @@
       <c r="H52" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I52" s="3"/>
-      <c r="J52" s="3" t="s">
+      <c r="I52" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="K52" s="3" t="s">
+      <c r="L52" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="L52" s="3" t="s">
+      <c r="M52" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="M52" s="3"/>
       <c r="N52" s="3"/>
-      <c r="O52" s="3" t="s">
+      <c r="O52" s="3"/>
+      <c r="P52" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="P52" s="3" t="s">
+      <c r="Q52" s="3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -6635,8 +6905,9 @@
       <c r="N53" s="3"/>
       <c r="O53" s="3"/>
       <c r="P53" s="3"/>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q53" s="3"/>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>96</v>
       </c>
@@ -6655,26 +6926,29 @@
       <c r="H54" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I54" s="4"/>
-      <c r="J54" s="4" t="s">
+      <c r="I54" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J54" s="4"/>
+      <c r="K54" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="K54" s="4" t="s">
+      <c r="L54" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="L54" s="4" t="s">
+      <c r="M54" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M54" s="4"/>
       <c r="N54" s="4"/>
-      <c r="O54" s="4" t="s">
+      <c r="O54" s="4"/>
+      <c r="P54" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="P54" s="4" t="s">
+      <c r="Q54" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>96</v>
       </c>
@@ -6693,26 +6967,29 @@
       <c r="H55" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I55" s="4"/>
-      <c r="J55" s="4" t="s">
+      <c r="I55" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J55" s="4"/>
+      <c r="K55" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="K55" s="4" t="s">
+      <c r="L55" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="L55" s="4" t="s">
+      <c r="M55" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="M55" s="4"/>
       <c r="N55" s="4"/>
-      <c r="O55" s="4" t="s">
+      <c r="O55" s="4"/>
+      <c r="P55" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="P55" s="4" t="s">
+      <c r="Q55" s="4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>96</v>
       </c>
@@ -6731,26 +7008,29 @@
       <c r="H56" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I56" s="4"/>
-      <c r="J56" s="4" t="s">
+      <c r="I56" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J56" s="4"/>
+      <c r="K56" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="K56" s="4" t="s">
+      <c r="L56" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="L56" s="4" t="s">
+      <c r="M56" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="M56" s="4"/>
       <c r="N56" s="4"/>
-      <c r="O56" s="4" t="s">
+      <c r="O56" s="4"/>
+      <c r="P56" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="P56" s="4" t="s">
+      <c r="Q56" s="4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>96</v>
       </c>
@@ -6769,26 +7049,29 @@
       <c r="H57" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I57" s="4"/>
-      <c r="J57" s="4" t="s">
+      <c r="I57" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J57" s="4"/>
+      <c r="K57" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="K57" s="4" t="s">
+      <c r="L57" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="L57" s="4" t="s">
+      <c r="M57" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="M57" s="4"/>
       <c r="N57" s="4"/>
-      <c r="O57" s="4" t="s">
+      <c r="O57" s="4"/>
+      <c r="P57" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="P57" s="4" t="s">
+      <c r="Q57" s="4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>96</v>
       </c>
@@ -6807,28 +7090,31 @@
       <c r="H58" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I58" s="4"/>
-      <c r="J58" s="4" t="s">
+      <c r="I58" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J58" s="4"/>
+      <c r="K58" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="K58" s="4" t="s">
+      <c r="L58" s="4" t="s">
         <v>215</v>
-      </c>
-      <c r="L58" s="4" t="s">
-        <v>9</v>
       </c>
       <c r="M58" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="N58" s="4"/>
-      <c r="O58" s="4" t="s">
+      <c r="N58" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O58" s="4"/>
+      <c r="P58" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="P58" s="4" t="s">
+      <c r="Q58" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
         <v>96</v>
       </c>
@@ -6845,30 +7131,33 @@
         <v>1</v>
       </c>
       <c r="H59" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I59" s="4"/>
-      <c r="J59" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I59" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J59" s="4"/>
+      <c r="K59" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="K59" s="4" t="s">
+      <c r="L59" s="4" t="s">
         <v>215</v>
-      </c>
-      <c r="L59" s="4" t="s">
-        <v>130</v>
       </c>
       <c r="M59" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="N59" s="4"/>
-      <c r="O59" s="4" t="s">
+      <c r="N59" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="O59" s="4"/>
+      <c r="P59" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="P59" s="4" t="s">
+      <c r="Q59" s="4" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -6885,8 +7174,9 @@
       <c r="N60" s="4"/>
       <c r="O60" s="4"/>
       <c r="P60" s="4"/>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q60" s="4"/>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>116</v>
       </c>
@@ -6905,26 +7195,29 @@
       <c r="H61" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I61" s="3"/>
-      <c r="J61" s="3" t="s">
+      <c r="I61" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J61" s="3"/>
+      <c r="K61" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="K61" s="3" t="s">
+      <c r="L61" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="L61" s="3" t="s">
+      <c r="M61" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="M61" s="3"/>
       <c r="N61" s="3"/>
-      <c r="O61" s="3" t="s">
+      <c r="O61" s="3"/>
+      <c r="P61" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="P61" s="3" t="s">
+      <c r="Q61" s="3" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -6941,8 +7234,9 @@
       <c r="N62" s="3"/>
       <c r="O62" s="3"/>
       <c r="P62" s="3"/>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q62" s="3"/>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
         <v>122</v>
       </c>
@@ -6963,26 +7257,29 @@
       <c r="H63" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I63" s="4"/>
-      <c r="J63" s="4" t="s">
+      <c r="I63" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J63" s="4"/>
+      <c r="K63" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="K63" s="4" t="s">
+      <c r="L63" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="L63" s="4" t="s">
+      <c r="M63" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="M63" s="4"/>
       <c r="N63" s="4"/>
-      <c r="O63" s="4" t="s">
+      <c r="O63" s="4"/>
+      <c r="P63" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="P63" s="4" t="s">
+      <c r="Q63" s="4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
         <v>122</v>
       </c>
@@ -7003,26 +7300,29 @@
       <c r="H64" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I64" s="4"/>
-      <c r="J64" s="4" t="s">
+      <c r="I64" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J64" s="4"/>
+      <c r="K64" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="K64" s="4" t="s">
+      <c r="L64" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="L64" s="4" t="s">
+      <c r="M64" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="M64" s="4"/>
       <c r="N64" s="4"/>
-      <c r="O64" s="4" t="s">
+      <c r="O64" s="4"/>
+      <c r="P64" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="P64" s="4" t="s">
+      <c r="Q64" s="4" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" s="4"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
@@ -7039,8 +7339,9 @@
       <c r="N65" s="4"/>
       <c r="O65" s="4"/>
       <c r="P65" s="4"/>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q65" s="4"/>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>67</v>
       </c>
@@ -7056,25 +7357,26 @@
         <v>135</v>
       </c>
       <c r="G66" s="3"/>
-      <c r="H66" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I66" s="3"/>
-      <c r="J66" s="3" t="s">
+      <c r="H66" s="3"/>
+      <c r="I66" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J66" s="3"/>
+      <c r="K66" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="K66" s="3"/>
       <c r="L66" s="3"/>
       <c r="M66" s="3"/>
       <c r="N66" s="3"/>
-      <c r="O66" s="3" t="s">
+      <c r="O66" s="3"/>
+      <c r="P66" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="P66" s="3" t="s">
+      <c r="Q66" s="3" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>67</v>
       </c>
@@ -7095,26 +7397,29 @@
       <c r="H67" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I67" s="3"/>
-      <c r="J67" s="3" t="s">
+      <c r="I67" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J67" s="3"/>
+      <c r="K67" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="K67" s="3" t="s">
+      <c r="L67" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="L67" s="3" t="s">
+      <c r="M67" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="M67" s="3"/>
       <c r="N67" s="3"/>
-      <c r="O67" s="3" t="s">
+      <c r="O67" s="3"/>
+      <c r="P67" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="P67" s="3" t="s">
+      <c r="Q67" s="3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>67</v>
       </c>
@@ -7135,26 +7440,29 @@
       <c r="H68" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="I68" s="3"/>
-      <c r="J68" s="3" t="s">
+      <c r="I68" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J68" s="3"/>
+      <c r="K68" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="K68" s="3" t="s">
+      <c r="L68" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="L68" s="3" t="s">
+      <c r="M68" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="M68" s="3"/>
       <c r="N68" s="3"/>
-      <c r="O68" s="3" t="s">
+      <c r="O68" s="3"/>
+      <c r="P68" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="P68" s="3" t="s">
+      <c r="Q68" s="3" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>67</v>
       </c>
@@ -7170,25 +7478,26 @@
         <v>76</v>
       </c>
       <c r="G69" s="3"/>
-      <c r="H69" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I69" s="3"/>
-      <c r="J69" s="3" t="s">
+      <c r="H69" s="3"/>
+      <c r="I69" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J69" s="3"/>
+      <c r="K69" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="K69" s="3"/>
       <c r="L69" s="3"/>
       <c r="M69" s="3"/>
       <c r="N69" s="3"/>
-      <c r="O69" s="3" t="s">
+      <c r="O69" s="3"/>
+      <c r="P69" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="P69" s="3" t="s">
+      <c r="Q69" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -7205,8 +7514,9 @@
       <c r="N70" s="3"/>
       <c r="O70" s="3"/>
       <c r="P70" s="3"/>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q70" s="3"/>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
         <v>76</v>
       </c>
@@ -7227,26 +7537,29 @@
       <c r="H71" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I71" s="4"/>
-      <c r="J71" s="4" t="s">
+      <c r="I71" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J71" s="4"/>
+      <c r="K71" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="K71" s="4" t="s">
+      <c r="L71" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="L71" s="4" t="s">
+      <c r="M71" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="M71" s="4"/>
       <c r="N71" s="4"/>
-      <c r="O71" s="4" t="s">
+      <c r="O71" s="4"/>
+      <c r="P71" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="P71" s="4" t="s">
+      <c r="Q71" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
         <v>76</v>
       </c>
@@ -7265,26 +7578,29 @@
       <c r="H72" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I72" s="4"/>
-      <c r="J72" s="4" t="s">
+      <c r="I72" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J72" s="4"/>
+      <c r="K72" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="K72" s="4" t="s">
+      <c r="L72" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="L72" s="4" t="s">
+      <c r="M72" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="M72" s="4"/>
       <c r="N72" s="4"/>
-      <c r="O72" s="4" t="s">
+      <c r="O72" s="4"/>
+      <c r="P72" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="P72" s="4" t="s">
+      <c r="Q72" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
         <v>76</v>
       </c>
@@ -7303,26 +7619,29 @@
       <c r="H73" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I73" s="4"/>
-      <c r="J73" s="4" t="s">
+      <c r="I73" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J73" s="4"/>
+      <c r="K73" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="K73" s="4" t="s">
+      <c r="L73" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="L73" s="4" t="s">
+      <c r="M73" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="M73" s="4"/>
       <c r="N73" s="4"/>
-      <c r="O73" s="4" t="s">
+      <c r="O73" s="4"/>
+      <c r="P73" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="P73" s="4" t="s">
+      <c r="Q73" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
         <v>76</v>
       </c>
@@ -7341,26 +7660,29 @@
       <c r="H74" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I74" s="4"/>
-      <c r="J74" s="4" t="s">
+      <c r="I74" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J74" s="4"/>
+      <c r="K74" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="K74" s="4" t="s">
+      <c r="L74" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="L74" s="4" t="s">
+      <c r="M74" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="M74" s="4"/>
       <c r="N74" s="4"/>
-      <c r="O74" s="4" t="s">
+      <c r="O74" s="4"/>
+      <c r="P74" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="P74" s="4" t="s">
+      <c r="Q74" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
         <v>76</v>
       </c>
@@ -7379,28 +7701,31 @@
       <c r="H75" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I75" s="4"/>
-      <c r="J75" s="4" t="s">
+      <c r="I75" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J75" s="4"/>
+      <c r="K75" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="K75" s="4" t="s">
+      <c r="L75" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="L75" s="4" t="s">
+      <c r="M75" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="M75" s="4"/>
       <c r="N75" s="4"/>
-      <c r="O75" s="4" t="s">
+      <c r="O75" s="4"/>
+      <c r="P75" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="P75" s="4" t="s">
+      <c r="Q75" s="4" t="s">
         <v>87</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A1:Q1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>